<commit_message>
fix 19 nov 23
</commit_message>
<xml_diff>
--- a/attendance-kelas 6.xlsx
+++ b/attendance-kelas 6.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="StudentGrade" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>DAFTAR HADIR</t>
   </si>
@@ -41,7 +41,7 @@
     <t>izin</t>
   </si>
   <si>
-    <t>tanpa keterangan</t>
+    <t>tanpa_keterangan</t>
   </si>
   <si>
     <t>catatan</t>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>MUHAMMAD ZHAFIR FERDIANSYAH ALTHAF</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>ATHA'ILAH NAFIS RAYKHAN</t>
@@ -548,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -559,7 +562,7 @@
         <v>2018002</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -569,6 +572,21 @@
       </c>
       <c r="E5">
         <v>87</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -576,7 +594,7 @@
         <v>2018003</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -586,6 +604,21 @@
       </c>
       <c r="E6">
         <v>88</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -593,7 +626,7 @@
         <v>2018004</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -603,6 +636,21 @@
       </c>
       <c r="E7">
         <v>89</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -610,7 +658,7 @@
         <v>2018005</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -620,6 +668,21 @@
       </c>
       <c r="E8">
         <v>90</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -627,7 +690,7 @@
         <v>2018006</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -637,6 +700,21 @@
       </c>
       <c r="E9">
         <v>91</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -644,7 +722,7 @@
         <v>2018007</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -654,6 +732,21 @@
       </c>
       <c r="E10">
         <v>92</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -661,7 +754,7 @@
         <v>2018008</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -671,6 +764,21 @@
       </c>
       <c r="E11">
         <v>93</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -678,7 +786,7 @@
         <v>2018009</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -688,6 +796,21 @@
       </c>
       <c r="E12">
         <v>94</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -695,7 +818,7 @@
         <v>2018010</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -705,6 +828,21 @@
       </c>
       <c r="E13">
         <v>95</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -712,7 +850,7 @@
         <v>2018011</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -722,6 +860,21 @@
       </c>
       <c r="E14">
         <v>96</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -729,7 +882,7 @@
         <v>2018012</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -739,6 +892,21 @@
       </c>
       <c r="E15">
         <v>97</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -746,7 +914,7 @@
         <v>2018013</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -756,6 +924,21 @@
       </c>
       <c r="E16">
         <v>98</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -763,7 +946,7 @@
         <v>2018014</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -773,6 +956,21 @@
       </c>
       <c r="E17">
         <v>99</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -780,7 +978,7 @@
         <v>2018015</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -790,6 +988,21 @@
       </c>
       <c r="E18">
         <v>100</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -797,7 +1010,7 @@
         <v>2018016</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -807,6 +1020,21 @@
       </c>
       <c r="E19">
         <v>101</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -814,7 +1042,7 @@
         <v>2018017</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -824,6 +1052,21 @@
       </c>
       <c r="E20">
         <v>102</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -831,7 +1074,7 @@
         <v>2018018</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -841,6 +1084,21 @@
       </c>
       <c r="E21">
         <v>103</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -848,7 +1106,7 @@
         <v>2018019</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -858,6 +1116,21 @@
       </c>
       <c r="E22">
         <v>104</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -865,7 +1138,7 @@
         <v>2018020</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -875,6 +1148,21 @@
       </c>
       <c r="E23">
         <v>105</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -882,7 +1170,7 @@
         <v>2018021</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -892,6 +1180,21 @@
       </c>
       <c r="E24">
         <v>106</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -899,7 +1202,7 @@
         <v>2018022</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -909,6 +1212,21 @@
       </c>
       <c r="E25">
         <v>107</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -916,7 +1234,7 @@
         <v>2018023</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -926,6 +1244,21 @@
       </c>
       <c r="E26">
         <v>108</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -933,7 +1266,7 @@
         <v>2018024</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -943,6 +1276,21 @@
       </c>
       <c r="E27">
         <v>109</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -950,7 +1298,7 @@
         <v>2018025</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -960,6 +1308,21 @@
       </c>
       <c r="E28">
         <v>110</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -967,7 +1330,7 @@
         <v>2018026</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -977,6 +1340,21 @@
       </c>
       <c r="E29">
         <v>111</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -984,7 +1362,7 @@
         <v>2018027</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -994,6 +1372,21 @@
       </c>
       <c r="E30">
         <v>112</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1001,7 +1394,7 @@
         <v>2018028</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1011,6 +1404,21 @@
       </c>
       <c r="E31">
         <v>113</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>